<commit_message>
Add finance ministers time line
</commit_message>
<xml_diff>
--- a/data/inflation-table.xlsx
+++ b/data/inflation-table.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\RepTemplates\data_analytics\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{083ED36C-D81E-4780-A592-91B24F21E5B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16205AA8-FDB9-4946-82A1-5B60BC3A98C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{BB64A6D5-33E3-4D2D-A2FB-A85CC3792D07}"/>
   </bookViews>
@@ -734,7 +734,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="16">
+  <fonts count="17">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -828,6 +828,11 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -1006,13 +1011,97 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" indent="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" indent="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" indent="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" indent="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" indent="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="5"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1023,9 +1112,6 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -1041,14 +1127,35 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="4"/>
@@ -1059,108 +1166,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="4"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" indent="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" indent="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" indent="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" indent="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" indent="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" shrinkToFit="1"/>
-    </xf>
+    <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1475,1534 +1481,1588 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D171CBEE-8DAC-456C-A30A-7A82A2FFE36E}">
-  <dimension ref="A1:T28"/>
+  <dimension ref="A1:T29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2"/>
   <cols>
-    <col min="1" max="1" width="10.44140625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="5.77734375" style="2" customWidth="1"/>
-    <col min="3" max="3" width="7.109375" style="2" customWidth="1"/>
-    <col min="4" max="5" width="5.77734375" style="2" customWidth="1"/>
-    <col min="6" max="6" width="6.88671875" style="2" customWidth="1"/>
-    <col min="7" max="7" width="5.77734375" style="2" customWidth="1"/>
-    <col min="8" max="8" width="7.109375" style="2" customWidth="1"/>
-    <col min="9" max="9" width="6.21875" style="2" customWidth="1"/>
-    <col min="10" max="10" width="6.88671875" style="2" customWidth="1"/>
-    <col min="11" max="11" width="6.6640625" style="2" customWidth="1"/>
-    <col min="12" max="14" width="5.77734375" style="2" customWidth="1"/>
-    <col min="15" max="15" width="5.5546875" style="2" customWidth="1"/>
-    <col min="16" max="16" width="7.109375" style="2" customWidth="1"/>
-    <col min="17" max="17" width="5.5546875" style="2" customWidth="1"/>
-    <col min="18" max="18" width="6.44140625" style="2" customWidth="1"/>
-    <col min="19" max="19" width="6.21875" style="2" customWidth="1"/>
-    <col min="20" max="20" width="2.88671875" style="2" customWidth="1"/>
-    <col min="21" max="16384" width="8.88671875" style="2"/>
+    <col min="1" max="1" width="10.44140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="5.77734375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="7.109375" style="1" customWidth="1"/>
+    <col min="4" max="5" width="5.77734375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="6.88671875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="5.77734375" style="1" customWidth="1"/>
+    <col min="8" max="8" width="7.109375" style="1" customWidth="1"/>
+    <col min="9" max="9" width="6.21875" style="1" customWidth="1"/>
+    <col min="10" max="10" width="6.88671875" style="1" customWidth="1"/>
+    <col min="11" max="11" width="6.6640625" style="1" customWidth="1"/>
+    <col min="12" max="14" width="5.77734375" style="1" customWidth="1"/>
+    <col min="15" max="15" width="5.5546875" style="1" customWidth="1"/>
+    <col min="16" max="16" width="7.109375" style="1" customWidth="1"/>
+    <col min="17" max="17" width="5.5546875" style="1" customWidth="1"/>
+    <col min="18" max="18" width="6.44140625" style="1" customWidth="1"/>
+    <col min="19" max="19" width="6.21875" style="1" customWidth="1"/>
+    <col min="20" max="20" width="2.88671875" style="1" customWidth="1"/>
+    <col min="21" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="315" customHeight="1">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
-      <c r="L1" s="1"/>
-      <c r="M1" s="1"/>
-      <c r="N1" s="1"/>
-      <c r="O1" s="1"/>
-      <c r="P1" s="1"/>
-      <c r="Q1" s="1"/>
-      <c r="R1" s="1"/>
-      <c r="S1" s="1"/>
-      <c r="T1" s="1"/>
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
+      <c r="G1" s="30"/>
+      <c r="H1" s="30"/>
+      <c r="I1" s="30"/>
+      <c r="J1" s="30"/>
+      <c r="K1" s="30"/>
+      <c r="L1" s="30"/>
+      <c r="M1" s="30"/>
+      <c r="N1" s="30"/>
+      <c r="O1" s="30"/>
+      <c r="P1" s="30"/>
+      <c r="Q1" s="30"/>
+      <c r="R1" s="30"/>
+      <c r="S1" s="30"/>
+      <c r="T1" s="30"/>
     </row>
     <row r="2" spans="1:20" ht="17.55" customHeight="1">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="4"/>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
-      <c r="I2" s="4"/>
-      <c r="J2" s="4"/>
-      <c r="K2" s="4"/>
-      <c r="L2" s="4"/>
-      <c r="M2" s="4"/>
-      <c r="N2" s="4"/>
-      <c r="O2" s="4"/>
-      <c r="P2" s="4"/>
-      <c r="Q2" s="4"/>
-      <c r="R2" s="4"/>
-      <c r="S2" s="5"/>
+      <c r="B2" s="32"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="32"/>
+      <c r="H2" s="32"/>
+      <c r="I2" s="32"/>
+      <c r="J2" s="32"/>
+      <c r="K2" s="32"/>
+      <c r="L2" s="32"/>
+      <c r="M2" s="32"/>
+      <c r="N2" s="32"/>
+      <c r="O2" s="32"/>
+      <c r="P2" s="32"/>
+      <c r="Q2" s="32"/>
+      <c r="R2" s="32"/>
+      <c r="S2" s="33"/>
     </row>
     <row r="3" spans="1:20" ht="12.75" customHeight="1">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="34" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="8"/>
-      <c r="D3" s="8"/>
-      <c r="E3" s="8"/>
-      <c r="F3" s="8"/>
-      <c r="G3" s="8"/>
-      <c r="H3" s="8"/>
-      <c r="I3" s="8"/>
-      <c r="J3" s="8"/>
-      <c r="K3" s="8"/>
-      <c r="L3" s="8"/>
-      <c r="M3" s="8"/>
-      <c r="N3" s="8"/>
-      <c r="O3" s="9"/>
-      <c r="P3" s="10" t="s">
+      <c r="C3" s="35"/>
+      <c r="D3" s="35"/>
+      <c r="E3" s="35"/>
+      <c r="F3" s="35"/>
+      <c r="G3" s="35"/>
+      <c r="H3" s="35"/>
+      <c r="I3" s="35"/>
+      <c r="J3" s="35"/>
+      <c r="K3" s="35"/>
+      <c r="L3" s="35"/>
+      <c r="M3" s="35"/>
+      <c r="N3" s="35"/>
+      <c r="O3" s="36"/>
+      <c r="P3" s="37" t="s">
         <v>4</v>
       </c>
-      <c r="Q3" s="11"/>
-      <c r="R3" s="12" t="s">
+      <c r="Q3" s="38"/>
+      <c r="R3" s="43" t="s">
         <v>5</v>
       </c>
-      <c r="S3" s="13"/>
+      <c r="S3" s="44"/>
     </row>
     <row r="4" spans="1:20" ht="12.75" customHeight="1">
-      <c r="A4" s="14"/>
-      <c r="B4" s="7" t="s">
+      <c r="A4" s="3"/>
+      <c r="B4" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="8"/>
-      <c r="D4" s="8"/>
-      <c r="E4" s="8"/>
-      <c r="F4" s="8"/>
-      <c r="G4" s="9"/>
-      <c r="H4" s="7" t="s">
+      <c r="C4" s="35"/>
+      <c r="D4" s="35"/>
+      <c r="E4" s="35"/>
+      <c r="F4" s="35"/>
+      <c r="G4" s="36"/>
+      <c r="H4" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="I4" s="8"/>
-      <c r="J4" s="8"/>
-      <c r="K4" s="9"/>
-      <c r="L4" s="15" t="s">
+      <c r="I4" s="35"/>
+      <c r="J4" s="35"/>
+      <c r="K4" s="36"/>
+      <c r="L4" s="49" t="s">
         <v>8</v>
       </c>
-      <c r="M4" s="16"/>
-      <c r="N4" s="16"/>
-      <c r="O4" s="17"/>
-      <c r="P4" s="18"/>
-      <c r="Q4" s="19"/>
-      <c r="R4" s="20"/>
-      <c r="S4" s="21"/>
+      <c r="M4" s="50"/>
+      <c r="N4" s="50"/>
+      <c r="O4" s="51"/>
+      <c r="P4" s="39"/>
+      <c r="Q4" s="40"/>
+      <c r="R4" s="45"/>
+      <c r="S4" s="46"/>
     </row>
     <row r="5" spans="1:20" ht="14.7" customHeight="1">
-      <c r="A5" s="14"/>
-      <c r="B5" s="22" t="s">
+      <c r="A5" s="3"/>
+      <c r="B5" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="23"/>
-      <c r="D5" s="22" t="s">
+      <c r="C5" s="29"/>
+      <c r="D5" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="E5" s="23"/>
-      <c r="F5" s="24" t="s">
+      <c r="E5" s="29"/>
+      <c r="F5" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="G5" s="25"/>
-      <c r="H5" s="24" t="s">
+      <c r="G5" s="27"/>
+      <c r="H5" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="I5" s="25"/>
-      <c r="J5" s="24" t="s">
+      <c r="I5" s="27"/>
+      <c r="J5" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="K5" s="25"/>
-      <c r="L5" s="22" t="s">
+      <c r="K5" s="27"/>
+      <c r="L5" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="M5" s="23"/>
-      <c r="N5" s="24" t="s">
+      <c r="M5" s="29"/>
+      <c r="N5" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="O5" s="25"/>
-      <c r="P5" s="26"/>
-      <c r="Q5" s="27"/>
-      <c r="R5" s="28"/>
-      <c r="S5" s="29"/>
+      <c r="O5" s="27"/>
+      <c r="P5" s="41"/>
+      <c r="Q5" s="42"/>
+      <c r="R5" s="47"/>
+      <c r="S5" s="48"/>
     </row>
     <row r="6" spans="1:20" ht="16.2" customHeight="1">
-      <c r="A6" s="30"/>
-      <c r="B6" s="31" t="s">
+      <c r="A6" s="4"/>
+      <c r="B6" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="32" t="s">
+      <c r="C6" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="D6" s="31" t="s">
+      <c r="D6" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E6" s="32" t="s">
+      <c r="E6" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="F6" s="32" t="s">
+      <c r="F6" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="G6" s="32" t="s">
+      <c r="G6" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="H6" s="31" t="s">
+      <c r="H6" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="I6" s="33" t="s">
+      <c r="I6" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="J6" s="31" t="s">
+      <c r="J6" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="K6" s="33" t="s">
+      <c r="K6" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="L6" s="31" t="s">
+      <c r="L6" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="M6" s="34" t="s">
+      <c r="M6" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="N6" s="31" t="s">
+      <c r="N6" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="O6" s="32" t="s">
+      <c r="O6" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="P6" s="31" t="s">
+      <c r="P6" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="Q6" s="32" t="s">
+      <c r="Q6" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="R6" s="34" t="s">
+      <c r="R6" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="S6" s="34" t="s">
+      <c r="S6" s="8" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:20" ht="15.75" customHeight="1">
-      <c r="A7" s="35" t="s">
+      <c r="A7" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="36">
+      <c r="B7" s="10">
         <v>9.6999999999999993</v>
       </c>
-      <c r="C7" s="37">
+      <c r="C7" s="11">
         <v>-0.3</v>
       </c>
-      <c r="D7" s="38">
+      <c r="D7" s="12">
         <v>9.6</v>
       </c>
-      <c r="E7" s="37">
+      <c r="E7" s="11">
         <v>-0.4</v>
       </c>
-      <c r="F7" s="37">
+      <c r="F7" s="11">
         <v>9.6999999999999993</v>
       </c>
-      <c r="G7" s="37">
+      <c r="G7" s="11">
         <v>-0.1</v>
       </c>
-      <c r="H7" s="38">
+      <c r="H7" s="12">
         <v>11</v>
       </c>
-      <c r="I7" s="36">
+      <c r="I7" s="10">
         <v>-1.9</v>
       </c>
-      <c r="J7" s="39">
+      <c r="J7" s="13">
         <v>9.8000000000000007</v>
       </c>
-      <c r="K7" s="36">
+      <c r="K7" s="10">
         <v>-0.8</v>
       </c>
-      <c r="L7" s="38">
+      <c r="L7" s="12">
         <v>8.8000000000000007</v>
       </c>
-      <c r="M7" s="36">
+      <c r="M7" s="10">
         <v>0.5</v>
       </c>
-      <c r="N7" s="36">
+      <c r="N7" s="10">
         <v>9.6999999999999993</v>
       </c>
-      <c r="O7" s="37">
+      <c r="O7" s="11">
         <v>0.6</v>
       </c>
-      <c r="P7" s="39">
+      <c r="P7" s="13">
         <v>17.600000000000001</v>
       </c>
-      <c r="Q7" s="37">
+      <c r="Q7" s="11">
         <v>-0.4</v>
       </c>
-      <c r="R7" s="36">
+      <c r="R7" s="10">
         <v>20.9</v>
       </c>
-      <c r="S7" s="40">
+      <c r="S7" s="14">
         <v>0.9</v>
       </c>
     </row>
     <row r="8" spans="1:20" ht="15.75" customHeight="1">
-      <c r="A8" s="35" t="s">
+      <c r="A8" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="36">
+      <c r="B8" s="10">
         <v>8.4</v>
       </c>
-      <c r="C8" s="37">
+      <c r="C8" s="11">
         <v>1.3</v>
       </c>
-      <c r="D8" s="38">
+      <c r="D8" s="12">
         <v>8.6999999999999993</v>
       </c>
-      <c r="E8" s="37">
+      <c r="E8" s="11">
         <v>1.3</v>
       </c>
-      <c r="F8" s="37">
+      <c r="F8" s="11">
         <v>8</v>
       </c>
-      <c r="G8" s="37">
+      <c r="G8" s="11">
         <v>1.4</v>
       </c>
-      <c r="H8" s="40">
+      <c r="H8" s="14">
         <v>9.4</v>
       </c>
-      <c r="I8" s="40">
+      <c r="I8" s="14">
         <v>1.5</v>
       </c>
-      <c r="J8" s="39">
+      <c r="J8" s="13">
         <v>7.3</v>
       </c>
-      <c r="K8" s="40">
+      <c r="K8" s="14">
         <v>1.6</v>
       </c>
-      <c r="L8" s="38">
+      <c r="L8" s="12">
         <v>8.1999999999999993</v>
       </c>
-      <c r="M8" s="36">
+      <c r="M8" s="10">
         <v>1.1000000000000001</v>
       </c>
-      <c r="N8" s="36">
+      <c r="N8" s="10">
         <v>8.6999999999999993</v>
       </c>
-      <c r="O8" s="37">
+      <c r="O8" s="11">
         <v>1.2</v>
       </c>
-      <c r="P8" s="39">
+      <c r="P8" s="13">
         <v>16.2</v>
       </c>
-      <c r="Q8" s="37">
+      <c r="Q8" s="11">
         <v>1.8</v>
       </c>
-      <c r="R8" s="36">
+      <c r="R8" s="10">
         <v>17.3</v>
       </c>
-      <c r="S8" s="40">
+      <c r="S8" s="14">
         <v>2.2999999999999998</v>
       </c>
     </row>
     <row r="9" spans="1:20" ht="15.75" customHeight="1">
-      <c r="A9" s="35" t="s">
+      <c r="A9" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="36">
+      <c r="B9" s="10">
         <v>8.4</v>
       </c>
-      <c r="C9" s="37">
+      <c r="C9" s="11">
         <v>0.6</v>
       </c>
-      <c r="D9" s="38">
+      <c r="D9" s="12">
         <v>8.3000000000000007</v>
       </c>
-      <c r="E9" s="37">
+      <c r="E9" s="11">
         <v>0.5</v>
       </c>
-      <c r="F9" s="37">
+      <c r="F9" s="11">
         <v>8.4</v>
       </c>
-      <c r="G9" s="37">
+      <c r="G9" s="11">
         <v>0.7</v>
       </c>
-      <c r="H9" s="38">
+      <c r="H9" s="12">
         <v>10.199999999999999</v>
       </c>
-      <c r="I9" s="40">
+      <c r="I9" s="14">
         <v>0.5</v>
       </c>
-      <c r="J9" s="39">
+      <c r="J9" s="13">
         <v>9.1</v>
       </c>
-      <c r="K9" s="40">
+      <c r="K9" s="14">
         <v>0.8</v>
       </c>
-      <c r="L9" s="38">
+      <c r="L9" s="12">
         <v>7.2</v>
       </c>
-      <c r="M9" s="36">
+      <c r="M9" s="10">
         <v>0.5</v>
       </c>
-      <c r="N9" s="36">
+      <c r="N9" s="10">
         <v>7.7</v>
       </c>
-      <c r="O9" s="37">
+      <c r="O9" s="11">
         <v>0.6</v>
       </c>
-      <c r="P9" s="39">
+      <c r="P9" s="13">
         <v>15.9</v>
       </c>
-      <c r="Q9" s="37">
+      <c r="Q9" s="11">
         <v>0.7</v>
       </c>
-      <c r="R9" s="36">
+      <c r="R9" s="10">
         <v>17.100000000000001</v>
       </c>
-      <c r="S9" s="40">
+      <c r="S9" s="14">
         <v>1.2</v>
       </c>
     </row>
     <row r="10" spans="1:20" ht="15.75" customHeight="1">
-      <c r="A10" s="35" t="s">
+      <c r="A10" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="36">
+      <c r="B10" s="10">
         <v>9</v>
       </c>
-      <c r="C10" s="37">
+      <c r="C10" s="11">
         <v>2.1</v>
       </c>
-      <c r="D10" s="38">
+      <c r="D10" s="12">
         <v>9.1</v>
       </c>
-      <c r="E10" s="37">
+      <c r="E10" s="11">
         <v>2</v>
       </c>
-      <c r="F10" s="37">
+      <c r="F10" s="11">
         <v>8.8000000000000007</v>
       </c>
-      <c r="G10" s="37">
+      <c r="G10" s="11">
         <v>2.2999999999999998</v>
       </c>
-      <c r="H10" s="38">
+      <c r="H10" s="12">
         <v>10.8</v>
       </c>
-      <c r="I10" s="40">
+      <c r="I10" s="14">
         <v>3.6</v>
       </c>
-      <c r="J10" s="39">
+      <c r="J10" s="13">
         <v>9.1</v>
       </c>
-      <c r="K10" s="40">
+      <c r="K10" s="14">
         <v>3.7</v>
       </c>
-      <c r="L10" s="38">
+      <c r="L10" s="12">
         <v>8.1</v>
       </c>
-      <c r="M10" s="36">
+      <c r="M10" s="10">
         <v>1.1000000000000001</v>
       </c>
-      <c r="N10" s="36">
+      <c r="N10" s="10">
         <v>8.5</v>
       </c>
-      <c r="O10" s="37">
+      <c r="O10" s="11">
         <v>1</v>
       </c>
-      <c r="P10" s="39">
+      <c r="P10" s="13">
         <v>16.600000000000001</v>
       </c>
-      <c r="Q10" s="37">
+      <c r="Q10" s="11">
         <v>2.7</v>
       </c>
-      <c r="R10" s="36">
+      <c r="R10" s="10">
         <v>19.600000000000001</v>
       </c>
-      <c r="S10" s="40">
+      <c r="S10" s="14">
         <v>3.2</v>
       </c>
     </row>
     <row r="11" spans="1:20" ht="15.75" customHeight="1">
-      <c r="A11" s="35" t="s">
+      <c r="A11" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="36">
+      <c r="B11" s="10">
         <v>9.1999999999999993</v>
       </c>
-      <c r="C11" s="37">
+      <c r="C11" s="11">
         <v>1.9</v>
       </c>
-      <c r="D11" s="38">
+      <c r="D11" s="12">
         <v>9.6</v>
       </c>
-      <c r="E11" s="37">
+      <c r="E11" s="11">
         <v>1.7</v>
       </c>
-      <c r="F11" s="37">
+      <c r="F11" s="11">
         <v>8.6999999999999993</v>
       </c>
-      <c r="G11" s="37">
+      <c r="G11" s="11">
         <v>2.2000000000000002</v>
       </c>
-      <c r="H11" s="40">
+      <c r="H11" s="14">
         <v>9.4</v>
       </c>
-      <c r="I11" s="40">
+      <c r="I11" s="14">
         <v>1.5</v>
       </c>
-      <c r="J11" s="39">
+      <c r="J11" s="13">
         <v>7.2</v>
       </c>
-      <c r="K11" s="40">
+      <c r="K11" s="14">
         <v>2.6</v>
       </c>
-      <c r="L11" s="38">
+      <c r="L11" s="12">
         <v>9.6999999999999993</v>
       </c>
-      <c r="M11" s="36">
+      <c r="M11" s="10">
         <v>1.8</v>
       </c>
-      <c r="N11" s="38">
+      <c r="N11" s="12">
         <v>10</v>
       </c>
-      <c r="O11" s="37">
+      <c r="O11" s="11">
         <v>1.9</v>
       </c>
-      <c r="P11" s="39">
+      <c r="P11" s="13">
         <v>15.2</v>
       </c>
-      <c r="Q11" s="37">
+      <c r="Q11" s="11">
         <v>2.1</v>
       </c>
-      <c r="R11" s="36">
+      <c r="R11" s="10">
         <v>21.2</v>
       </c>
-      <c r="S11" s="40">
+      <c r="S11" s="14">
         <v>4.2</v>
       </c>
     </row>
     <row r="12" spans="1:20" ht="16.5" customHeight="1">
-      <c r="A12" s="41" t="s">
+      <c r="A12" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="B12" s="42">
+      <c r="B12" s="16">
         <v>11.5</v>
       </c>
-      <c r="C12" s="43">
+      <c r="C12" s="17">
         <v>3</v>
       </c>
-      <c r="D12" s="42">
+      <c r="D12" s="16">
         <v>12</v>
       </c>
-      <c r="E12" s="43">
+      <c r="E12" s="17">
         <v>2.9</v>
       </c>
-      <c r="F12" s="43">
+      <c r="F12" s="17">
         <v>10.9</v>
       </c>
-      <c r="G12" s="43">
+      <c r="G12" s="17">
         <v>3.1</v>
       </c>
-      <c r="H12" s="42">
+      <c r="H12" s="16">
         <v>11.9</v>
       </c>
-      <c r="I12" s="44">
+      <c r="I12" s="18">
         <v>3.9</v>
       </c>
-      <c r="J12" s="45">
+      <c r="J12" s="19">
         <v>8.6</v>
       </c>
-      <c r="K12" s="44">
+      <c r="K12" s="18">
         <v>3.3</v>
       </c>
-      <c r="L12" s="42">
+      <c r="L12" s="16">
         <v>12</v>
       </c>
-      <c r="M12" s="46">
+      <c r="M12" s="20">
         <v>2.2000000000000002</v>
       </c>
-      <c r="N12" s="42">
+      <c r="N12" s="16">
         <v>13</v>
       </c>
-      <c r="O12" s="43">
+      <c r="O12" s="17">
         <v>3</v>
       </c>
-      <c r="P12" s="42">
+      <c r="P12" s="16">
         <v>18.100000000000001</v>
       </c>
-      <c r="Q12" s="43">
+      <c r="Q12" s="17">
         <v>3.6</v>
       </c>
-      <c r="R12" s="46">
+      <c r="R12" s="20">
         <v>27</v>
       </c>
-      <c r="S12" s="46">
+      <c r="S12" s="20">
         <v>3.8</v>
       </c>
     </row>
     <row r="13" spans="1:20" ht="16.5" customHeight="1">
-      <c r="A13" s="41" t="s">
+      <c r="A13" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="B13" s="42">
+      <c r="B13" s="16">
         <v>12.3</v>
       </c>
-      <c r="C13" s="43">
+      <c r="C13" s="17">
         <v>0</v>
       </c>
-      <c r="D13" s="42">
+      <c r="D13" s="16">
         <v>12.7</v>
       </c>
-      <c r="E13" s="43">
+      <c r="E13" s="17">
         <v>0.3</v>
       </c>
-      <c r="F13" s="43">
+      <c r="F13" s="17">
         <v>11.6</v>
       </c>
-      <c r="G13" s="43">
+      <c r="G13" s="17">
         <v>-0.5</v>
       </c>
-      <c r="H13" s="42">
+      <c r="H13" s="16">
         <v>11.7</v>
       </c>
-      <c r="I13" s="46">
+      <c r="I13" s="20">
         <v>-2.2999999999999998</v>
       </c>
-      <c r="J13" s="45">
+      <c r="J13" s="19">
         <v>9</v>
       </c>
-      <c r="K13" s="46">
+      <c r="K13" s="20">
         <v>-3.1</v>
       </c>
-      <c r="L13" s="42">
+      <c r="L13" s="16">
         <v>13.4</v>
       </c>
-      <c r="M13" s="46">
+      <c r="M13" s="20">
         <v>2</v>
       </c>
-      <c r="N13" s="42">
+      <c r="N13" s="16">
         <v>14</v>
       </c>
-      <c r="O13" s="43">
+      <c r="O13" s="17">
         <v>1.9</v>
       </c>
-      <c r="P13" s="42">
+      <c r="P13" s="16">
         <v>20.9</v>
       </c>
-      <c r="Q13" s="43">
+      <c r="Q13" s="17">
         <v>-0.4</v>
       </c>
-      <c r="R13" s="46">
+      <c r="R13" s="20">
         <v>26.2</v>
       </c>
-      <c r="S13" s="46">
+      <c r="S13" s="20">
         <v>-0.2</v>
       </c>
     </row>
     <row r="14" spans="1:20" ht="16.5" customHeight="1">
-      <c r="A14" s="41" t="s">
+      <c r="A14" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="B14" s="42">
+      <c r="B14" s="16">
         <v>13</v>
       </c>
-      <c r="C14" s="43">
+      <c r="C14" s="17">
         <v>0.4</v>
       </c>
-      <c r="D14" s="42">
+      <c r="D14" s="16">
         <v>13</v>
       </c>
-      <c r="E14" s="43">
+      <c r="E14" s="17">
         <v>0.1</v>
       </c>
-      <c r="F14" s="43">
+      <c r="F14" s="17">
         <v>12.9</v>
       </c>
-      <c r="G14" s="43">
+      <c r="G14" s="17">
         <v>0.9</v>
       </c>
-      <c r="H14" s="42">
+      <c r="H14" s="16">
         <v>13.3</v>
       </c>
-      <c r="I14" s="46">
+      <c r="I14" s="20">
         <v>-0.8</v>
       </c>
-      <c r="J14" s="42">
+      <c r="J14" s="16">
         <v>11.8</v>
       </c>
-      <c r="K14" s="44">
+      <c r="K14" s="18">
         <v>0.4</v>
       </c>
-      <c r="L14" s="42">
+      <c r="L14" s="16">
         <v>12.8</v>
       </c>
-      <c r="M14" s="46">
+      <c r="M14" s="20">
         <v>0.6</v>
       </c>
-      <c r="N14" s="42">
+      <c r="N14" s="16">
         <v>13.9</v>
       </c>
-      <c r="O14" s="43">
+      <c r="O14" s="17">
         <v>1.4</v>
       </c>
-      <c r="P14" s="42">
+      <c r="P14" s="16">
         <v>20.9</v>
       </c>
-      <c r="Q14" s="43">
+      <c r="Q14" s="17">
         <v>-0.8</v>
       </c>
-      <c r="R14" s="46">
+      <c r="R14" s="20">
         <v>24</v>
       </c>
-      <c r="S14" s="46">
+      <c r="S14" s="20">
         <v>0.6</v>
       </c>
     </row>
     <row r="15" spans="1:20" ht="16.5" customHeight="1">
-      <c r="A15" s="41" t="s">
+      <c r="A15" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="B15" s="42">
+      <c r="B15" s="16">
         <v>12.2</v>
       </c>
-      <c r="C15" s="43">
+      <c r="C15" s="17">
         <v>1.2</v>
       </c>
-      <c r="D15" s="42">
+      <c r="D15" s="16">
         <v>11.5</v>
       </c>
-      <c r="E15" s="43">
+      <c r="E15" s="17">
         <v>0.9</v>
       </c>
-      <c r="F15" s="43">
+      <c r="F15" s="17">
         <v>13.3</v>
       </c>
-      <c r="G15" s="43">
+      <c r="G15" s="17">
         <v>1.5</v>
       </c>
-      <c r="H15" s="42">
+      <c r="H15" s="16">
         <v>14.3</v>
       </c>
-      <c r="I15" s="44">
+      <c r="I15" s="18">
         <v>2.2000000000000002</v>
       </c>
-      <c r="J15" s="42">
+      <c r="J15" s="16">
         <v>14.6</v>
       </c>
-      <c r="K15" s="44">
+      <c r="K15" s="18">
         <v>2.6</v>
       </c>
-      <c r="L15" s="42">
+      <c r="L15" s="16">
         <v>9.9</v>
       </c>
-      <c r="M15" s="46">
+      <c r="M15" s="20">
         <v>0.2</v>
       </c>
-      <c r="N15" s="42">
+      <c r="N15" s="16">
         <v>12.2</v>
       </c>
-      <c r="O15" s="43">
+      <c r="O15" s="17">
         <v>0.4</v>
       </c>
-      <c r="P15" s="42">
+      <c r="P15" s="16">
         <v>18.7</v>
       </c>
-      <c r="Q15" s="43">
+      <c r="Q15" s="17">
         <v>1.3</v>
       </c>
-      <c r="R15" s="46">
+      <c r="R15" s="20">
         <v>23.6</v>
       </c>
-      <c r="S15" s="46">
+      <c r="S15" s="20">
         <v>1.9</v>
       </c>
     </row>
     <row r="16" spans="1:20" ht="16.5" customHeight="1">
-      <c r="A16" s="47" t="s">
+      <c r="A16" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="B16" s="48">
+      <c r="B16" s="22">
         <v>12.7</v>
       </c>
-      <c r="C16" s="49">
+      <c r="C16" s="23">
         <v>0.8</v>
       </c>
-      <c r="D16" s="48">
+      <c r="D16" s="22">
         <v>11.9</v>
       </c>
-      <c r="E16" s="49">
+      <c r="E16" s="23">
         <v>0.7</v>
       </c>
-      <c r="F16" s="49">
+      <c r="F16" s="23">
         <v>13.9</v>
       </c>
-      <c r="G16" s="49">
+      <c r="G16" s="23">
         <v>1</v>
       </c>
-      <c r="H16" s="48">
+      <c r="H16" s="22">
         <v>14.5</v>
       </c>
-      <c r="I16" s="50">
+      <c r="I16" s="24">
         <v>1.8</v>
       </c>
-      <c r="J16" s="48">
+      <c r="J16" s="22">
         <v>15.5</v>
       </c>
-      <c r="K16" s="50">
+      <c r="K16" s="24">
         <v>2.2999999999999998</v>
       </c>
-      <c r="L16" s="48">
+      <c r="L16" s="22">
         <v>10.4</v>
       </c>
-      <c r="M16" s="51">
+      <c r="M16" s="25">
         <v>-0.1</v>
       </c>
-      <c r="N16" s="48">
+      <c r="N16" s="22">
         <v>12.5</v>
       </c>
-      <c r="O16" s="49">
+      <c r="O16" s="23">
         <v>-0.2</v>
       </c>
-      <c r="P16" s="48">
+      <c r="P16" s="22">
         <v>13</v>
       </c>
-      <c r="Q16" s="49">
+      <c r="Q16" s="23">
         <v>0.6</v>
       </c>
-      <c r="R16" s="51">
+      <c r="R16" s="25">
         <v>23.8</v>
       </c>
-      <c r="S16" s="51">
+      <c r="S16" s="25">
         <v>3.9</v>
       </c>
     </row>
     <row r="17" spans="1:19" ht="16.5" customHeight="1">
-      <c r="A17" s="41" t="s">
+      <c r="A17" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="B17" s="42">
+      <c r="B17" s="16">
         <v>13.4</v>
       </c>
-      <c r="C17" s="43">
+      <c r="C17" s="17">
         <v>1.6</v>
       </c>
-      <c r="D17" s="42">
+      <c r="D17" s="16">
         <v>12.2</v>
       </c>
-      <c r="E17" s="43">
+      <c r="E17" s="17">
         <v>1.6</v>
       </c>
-      <c r="F17" s="43">
+      <c r="F17" s="17">
         <v>15.1</v>
       </c>
-      <c r="G17" s="43">
+      <c r="G17" s="17">
         <v>1.6</v>
       </c>
-      <c r="H17" s="42">
+      <c r="H17" s="16">
         <v>15.6</v>
       </c>
-      <c r="I17" s="44">
+      <c r="I17" s="18">
         <v>3.7</v>
       </c>
-      <c r="J17" s="42">
+      <c r="J17" s="16">
         <v>17.7</v>
       </c>
-      <c r="K17" s="44">
+      <c r="K17" s="18">
         <v>2.8</v>
       </c>
-      <c r="L17" s="42">
+      <c r="L17" s="16">
         <v>10.199999999999999</v>
       </c>
-      <c r="M17" s="46">
+      <c r="M17" s="20">
         <v>0.3</v>
       </c>
-      <c r="N17" s="42">
+      <c r="N17" s="16">
         <v>12.8</v>
       </c>
-      <c r="O17" s="43">
+      <c r="O17" s="17">
         <v>0.5</v>
       </c>
-      <c r="P17" s="42">
+      <c r="P17" s="16">
         <v>14.2</v>
       </c>
-      <c r="Q17" s="43">
+      <c r="Q17" s="17">
         <v>1.5</v>
       </c>
-      <c r="R17" s="46">
+      <c r="R17" s="20">
         <v>28.1</v>
       </c>
-      <c r="S17" s="46">
+      <c r="S17" s="20">
         <v>3.2</v>
       </c>
     </row>
     <row r="18" spans="1:19" ht="16.5" customHeight="1">
-      <c r="A18" s="41" t="s">
+      <c r="A18" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="B18" s="42">
+      <c r="B18" s="16">
         <v>13.8</v>
       </c>
-      <c r="C18" s="43">
+      <c r="C18" s="17">
         <v>0.4</v>
       </c>
-      <c r="D18" s="42">
+      <c r="D18" s="16">
         <v>12.4</v>
       </c>
-      <c r="E18" s="43">
+      <c r="E18" s="17">
         <v>0.3</v>
       </c>
-      <c r="F18" s="43">
+      <c r="F18" s="17">
         <v>15.9</v>
       </c>
-      <c r="G18" s="43">
+      <c r="G18" s="17">
         <v>0.6</v>
       </c>
-      <c r="H18" s="42">
+      <c r="H18" s="16">
         <v>15.5</v>
       </c>
-      <c r="I18" s="44">
+      <c r="I18" s="18">
         <v>1</v>
       </c>
-      <c r="J18" s="42">
+      <c r="J18" s="16">
         <v>19</v>
       </c>
-      <c r="K18" s="44">
+      <c r="K18" s="18">
         <v>1.3</v>
       </c>
-      <c r="L18" s="42">
+      <c r="L18" s="16">
         <v>10.4</v>
       </c>
-      <c r="M18" s="46">
+      <c r="M18" s="20">
         <v>-0.1</v>
       </c>
-      <c r="N18" s="42">
+      <c r="N18" s="16">
         <v>13.1</v>
       </c>
-      <c r="O18" s="43">
+      <c r="O18" s="17">
         <v>0</v>
       </c>
-      <c r="P18" s="42">
+      <c r="P18" s="16">
         <v>14.1</v>
       </c>
-      <c r="Q18" s="43">
+      <c r="Q18" s="17">
         <v>0.6</v>
       </c>
-      <c r="R18" s="46">
+      <c r="R18" s="20">
         <v>29.6</v>
       </c>
-      <c r="S18" s="46">
+      <c r="S18" s="20">
         <v>1.4</v>
       </c>
     </row>
     <row r="19" spans="1:19" ht="16.5" customHeight="1">
-      <c r="A19" s="41" t="s">
+      <c r="A19" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="B19" s="42">
+      <c r="B19" s="16">
         <v>21.3</v>
       </c>
-      <c r="C19" s="43">
+      <c r="C19" s="17">
         <v>6.3</v>
       </c>
-      <c r="D19" s="42">
+      <c r="D19" s="16">
         <v>19.8</v>
       </c>
-      <c r="E19" s="43">
+      <c r="E19" s="17">
         <v>6.2</v>
       </c>
-      <c r="F19" s="43">
+      <c r="F19" s="17">
         <v>23.6</v>
       </c>
-      <c r="G19" s="43">
+      <c r="G19" s="17">
         <v>6.6</v>
       </c>
-      <c r="H19" s="42">
+      <c r="H19" s="16">
         <v>24</v>
       </c>
-      <c r="I19" s="44">
+      <c r="I19" s="18">
         <v>5.3</v>
       </c>
-      <c r="J19" s="42">
+      <c r="J19" s="16">
         <v>27</v>
       </c>
-      <c r="K19" s="44">
+      <c r="K19" s="18">
         <v>6</v>
       </c>
-      <c r="L19" s="42">
+      <c r="L19" s="16">
         <v>17.3</v>
       </c>
-      <c r="M19" s="46">
+      <c r="M19" s="20">
         <v>6.8</v>
       </c>
-      <c r="N19" s="42">
+      <c r="N19" s="16">
         <v>20.399999999999999</v>
       </c>
-      <c r="O19" s="43">
+      <c r="O19" s="17">
         <v>7.1</v>
       </c>
-      <c r="P19" s="42">
+      <c r="P19" s="16">
         <v>21.7</v>
       </c>
-      <c r="Q19" s="43">
+      <c r="Q19" s="17">
         <v>6.2</v>
       </c>
-      <c r="R19" s="46">
+      <c r="R19" s="20">
         <v>38.9</v>
       </c>
-      <c r="S19" s="46">
+      <c r="S19" s="20">
         <v>8.1999999999999993</v>
       </c>
     </row>
     <row r="20" spans="1:19" ht="16.5" customHeight="1">
-      <c r="A20" s="41" t="s">
+      <c r="A20" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="B20" s="42">
+      <c r="B20" s="16">
         <v>24.9</v>
       </c>
-      <c r="C20" s="43">
+      <c r="C20" s="17">
         <v>4.3</v>
       </c>
-      <c r="D20" s="42">
+      <c r="D20" s="16">
         <v>23.6</v>
       </c>
-      <c r="E20" s="43">
+      <c r="E20" s="17">
         <v>4.5</v>
       </c>
-      <c r="F20" s="43">
+      <c r="F20" s="17">
         <v>26.9</v>
       </c>
-      <c r="G20" s="43">
+      <c r="G20" s="17">
         <v>4.2</v>
       </c>
-      <c r="H20" s="42">
+      <c r="H20" s="16">
         <v>27.4</v>
       </c>
-      <c r="I20" s="44">
+      <c r="I20" s="18">
         <v>4.3</v>
       </c>
-      <c r="J20" s="42">
+      <c r="J20" s="16">
         <v>29.6</v>
       </c>
-      <c r="K20" s="44">
+      <c r="K20" s="18">
         <v>3.7</v>
       </c>
-      <c r="L20" s="42">
+      <c r="L20" s="16">
         <v>21.3</v>
       </c>
-      <c r="M20" s="46">
+      <c r="M20" s="20">
         <v>4.5999999999999996</v>
       </c>
-      <c r="N20" s="42">
+      <c r="N20" s="16">
         <v>24.5</v>
       </c>
-      <c r="O20" s="43">
+      <c r="O20" s="17">
         <v>4.5999999999999996</v>
       </c>
-      <c r="P20" s="42">
+      <c r="P20" s="16">
         <v>28.2</v>
       </c>
-      <c r="Q20" s="43">
+      <c r="Q20" s="17">
         <v>7.3</v>
       </c>
-      <c r="R20" s="46">
+      <c r="R20" s="20">
         <v>38.5</v>
       </c>
-      <c r="S20" s="46">
+      <c r="S20" s="20">
         <v>2</v>
       </c>
     </row>
     <row r="21" spans="1:19" ht="16.5" customHeight="1">
-      <c r="A21" s="41" t="s">
+      <c r="A21" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="B21" s="42">
+      <c r="B21" s="16">
         <v>27.3</v>
       </c>
-      <c r="C21" s="43">
+      <c r="C21" s="17">
         <v>2.4</v>
       </c>
-      <c r="D21" s="42">
+      <c r="D21" s="16">
         <v>26.2</v>
       </c>
-      <c r="E21" s="43">
+      <c r="E21" s="17">
         <v>2.6</v>
       </c>
-      <c r="F21" s="43">
+      <c r="F21" s="17">
         <v>28.8</v>
       </c>
-      <c r="G21" s="43">
+      <c r="G21" s="17">
         <v>2.2000000000000002</v>
       </c>
-      <c r="H21" s="42">
+      <c r="H21" s="16">
         <v>28.8</v>
       </c>
-      <c r="I21" s="44">
+      <c r="I21" s="18">
         <v>1.6</v>
       </c>
-      <c r="J21" s="42">
+      <c r="J21" s="16">
         <v>30.2</v>
       </c>
-      <c r="K21" s="44">
+      <c r="K21" s="18">
         <v>1.2</v>
       </c>
-      <c r="L21" s="42">
+      <c r="L21" s="16">
         <v>24.7</v>
       </c>
-      <c r="M21" s="46">
+      <c r="M21" s="20">
         <v>3.3</v>
       </c>
-      <c r="N21" s="42">
+      <c r="N21" s="16">
         <v>27.5</v>
       </c>
-      <c r="O21" s="43">
+      <c r="O21" s="17">
         <v>3.1</v>
       </c>
-      <c r="P21" s="42">
+      <c r="P21" s="16">
         <v>34</v>
       </c>
-      <c r="Q21" s="43">
+      <c r="Q21" s="17">
         <v>5.2</v>
       </c>
-      <c r="R21" s="46">
+      <c r="R21" s="20">
         <v>41.2</v>
       </c>
-      <c r="S21" s="46">
+      <c r="S21" s="20">
         <v>3.1</v>
       </c>
     </row>
     <row r="22" spans="1:19" ht="20.25" customHeight="1">
-      <c r="A22" s="41" t="s">
+      <c r="A22" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="B22" s="42">
+      <c r="B22" s="16">
         <v>23.2</v>
       </c>
-      <c r="C22" s="43">
+      <c r="C22" s="17">
         <v>-1.2</v>
       </c>
-      <c r="D22" s="42">
+      <c r="D22" s="16">
         <v>21.2</v>
       </c>
-      <c r="E22" s="43">
+      <c r="E22" s="17">
         <v>-2.1</v>
       </c>
-      <c r="F22" s="43">
+      <c r="F22" s="17">
         <v>26.1</v>
       </c>
-      <c r="G22" s="43">
+      <c r="G22" s="17">
         <v>0.2</v>
       </c>
-      <c r="H22" s="42">
+      <c r="H22" s="16">
         <v>30.8</v>
       </c>
-      <c r="I22" s="44">
+      <c r="I22" s="18">
         <v>5.2</v>
       </c>
-      <c r="J22" s="42">
+      <c r="J22" s="16">
         <v>32.700000000000003</v>
       </c>
-      <c r="K22" s="44">
+      <c r="K22" s="18">
         <v>5.7</v>
       </c>
-      <c r="L22" s="42">
+      <c r="L22" s="16">
         <v>15.2</v>
       </c>
-      <c r="M22" s="46">
+      <c r="M22" s="20">
         <v>-6.6</v>
       </c>
-      <c r="N22" s="42">
+      <c r="N22" s="16">
         <v>20.100000000000001</v>
       </c>
-      <c r="O22" s="43">
+      <c r="O22" s="17">
         <v>-4.9000000000000004</v>
       </c>
-      <c r="P22" s="42">
+      <c r="P22" s="16">
         <v>28.6</v>
       </c>
-      <c r="Q22" s="43">
+      <c r="Q22" s="17">
         <v>-1.4</v>
       </c>
-      <c r="R22" s="46">
+      <c r="R22" s="20">
         <v>38.9</v>
       </c>
-      <c r="S22" s="46">
+      <c r="S22" s="20">
         <v>1.4</v>
       </c>
     </row>
     <row r="23" spans="1:19" ht="16.5" customHeight="1">
-      <c r="A23" s="41" t="s">
+      <c r="A23" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="B23" s="42">
+      <c r="B23" s="16">
         <v>26.6</v>
       </c>
-      <c r="C23" s="43">
+      <c r="C23" s="17">
         <v>4.7</v>
       </c>
-      <c r="D23" s="42">
+      <c r="D23" s="16">
         <v>24.6</v>
       </c>
-      <c r="E23" s="43">
+      <c r="E23" s="17">
         <v>4.5</v>
       </c>
-      <c r="F23" s="43">
+      <c r="F23" s="17">
         <v>29.5</v>
       </c>
-      <c r="G23" s="43">
+      <c r="G23" s="17">
         <v>5</v>
       </c>
-      <c r="H23" s="42">
+      <c r="H23" s="16">
         <v>34.700000000000003</v>
       </c>
-      <c r="I23" s="44">
+      <c r="I23" s="18">
         <v>4.5</v>
       </c>
-      <c r="J23" s="42">
+      <c r="J23" s="16">
         <v>37.200000000000003</v>
       </c>
-      <c r="K23" s="44">
+      <c r="K23" s="18">
         <v>6.1</v>
       </c>
-      <c r="L23" s="42">
+      <c r="L23" s="16">
         <v>18.2</v>
       </c>
-      <c r="M23" s="46">
+      <c r="M23" s="20">
         <v>4.5</v>
       </c>
-      <c r="N23" s="42">
+      <c r="N23" s="16">
         <v>22.4</v>
       </c>
-      <c r="O23" s="43">
+      <c r="O23" s="17">
         <v>3.9</v>
       </c>
-      <c r="P23" s="42">
+      <c r="P23" s="16">
         <v>24</v>
       </c>
-      <c r="Q23" s="43">
+      <c r="Q23" s="17">
         <v>-1.5</v>
       </c>
-      <c r="R23" s="46">
+      <c r="R23" s="20">
         <v>32.6</v>
       </c>
-      <c r="S23" s="46">
+      <c r="S23" s="20">
         <v>-0.5</v>
       </c>
     </row>
     <row r="24" spans="1:19" ht="17.55" customHeight="1">
-      <c r="A24" s="41" t="s">
+      <c r="A24" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="B24" s="42">
+      <c r="B24" s="16">
         <v>23.8</v>
       </c>
-      <c r="C24" s="43">
+      <c r="C24" s="17">
         <v>0.8</v>
       </c>
-      <c r="D24" s="42">
+      <c r="D24" s="16">
         <v>21.6</v>
       </c>
-      <c r="E24" s="43">
+      <c r="E24" s="17">
         <v>0.4</v>
       </c>
-      <c r="F24" s="43">
+      <c r="F24" s="17">
         <v>27.2</v>
       </c>
-      <c r="G24" s="43">
+      <c r="G24" s="17">
         <v>1.3</v>
       </c>
-      <c r="H24" s="42">
+      <c r="H24" s="16">
         <v>29.7</v>
       </c>
-      <c r="I24" s="44">
+      <c r="I24" s="18">
         <v>0</v>
       </c>
-      <c r="J24" s="42">
+      <c r="J24" s="16">
         <v>33.5</v>
       </c>
-      <c r="K24" s="44">
+      <c r="K24" s="18">
         <v>0.5</v>
       </c>
-      <c r="L24" s="42">
+      <c r="L24" s="16">
         <v>16.399999999999999</v>
       </c>
-      <c r="M24" s="46">
+      <c r="M24" s="20">
         <v>0.6</v>
       </c>
-      <c r="N24" s="42">
+      <c r="N24" s="16">
         <v>21.4</v>
       </c>
-      <c r="O24" s="43">
+      <c r="O24" s="17">
         <v>2.1</v>
       </c>
-      <c r="P24" s="42">
+      <c r="P24" s="16">
         <v>27.1</v>
       </c>
-      <c r="Q24" s="43">
+      <c r="Q24" s="17">
         <v>6.1</v>
       </c>
-      <c r="R24" s="46">
+      <c r="R24" s="20">
         <v>27.7</v>
       </c>
-      <c r="S24" s="46">
+      <c r="S24" s="20">
         <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:19" ht="20.25" customHeight="1">
-      <c r="A25" s="41" t="s">
+      <c r="A25" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="B25" s="42">
+      <c r="B25" s="16">
         <v>24.5</v>
       </c>
-      <c r="C25" s="43">
+      <c r="C25" s="17">
         <v>0.5</v>
       </c>
-      <c r="D25" s="42">
+      <c r="D25" s="16">
         <v>21.6</v>
       </c>
-      <c r="E25" s="43">
+      <c r="E25" s="17">
         <v>0.3</v>
       </c>
-      <c r="F25" s="43">
+      <c r="F25" s="17">
         <v>28.8</v>
       </c>
-      <c r="G25" s="43">
+      <c r="G25" s="17">
         <v>0.7</v>
       </c>
-      <c r="H25" s="42">
+      <c r="H25" s="16">
         <v>32.700000000000003</v>
       </c>
-      <c r="I25" s="44">
+      <c r="I25" s="18">
         <v>0</v>
       </c>
-      <c r="J25" s="42">
+      <c r="J25" s="16">
         <v>37.9</v>
       </c>
-      <c r="K25" s="44">
+      <c r="K25" s="18">
         <v>0.1</v>
       </c>
-      <c r="L25" s="42">
+      <c r="L25" s="16">
         <v>14.8</v>
       </c>
-      <c r="M25" s="46">
+      <c r="M25" s="20">
         <v>0.6</v>
       </c>
-      <c r="N25" s="42">
+      <c r="N25" s="16">
         <v>20.7</v>
       </c>
-      <c r="O25" s="43">
+      <c r="O25" s="17">
         <v>1.4</v>
       </c>
-      <c r="P25" s="42">
+      <c r="P25" s="16">
         <v>27.8</v>
       </c>
-      <c r="Q25" s="43">
+      <c r="Q25" s="17">
         <v>0.2</v>
       </c>
-      <c r="R25" s="46">
+      <c r="R25" s="20">
         <v>27.1</v>
       </c>
-      <c r="S25" s="46">
+      <c r="S25" s="20">
         <v>-0.7</v>
       </c>
     </row>
     <row r="26" spans="1:19" ht="20.25" customHeight="1">
-      <c r="A26" s="41" t="s">
+      <c r="A26" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="B26" s="42">
+      <c r="B26" s="16">
         <v>27.6</v>
       </c>
-      <c r="C26" s="43">
+      <c r="C26" s="17">
         <v>2.9</v>
       </c>
-      <c r="D26" s="42">
+      <c r="D26" s="16">
         <v>24.4</v>
       </c>
-      <c r="E26" s="43">
+      <c r="E26" s="17">
         <v>2.4</v>
       </c>
-      <c r="F26" s="43">
+      <c r="F26" s="17">
         <v>32.299999999999997</v>
       </c>
-      <c r="G26" s="43">
+      <c r="G26" s="17">
         <v>3.6</v>
       </c>
-      <c r="H26" s="42">
+      <c r="H26" s="16">
         <v>39</v>
       </c>
-      <c r="I26" s="44">
+      <c r="I26" s="18">
         <v>3.9</v>
       </c>
-      <c r="J26" s="42">
+      <c r="J26" s="16">
         <v>45.2</v>
       </c>
-      <c r="K26" s="44">
+      <c r="K26" s="18">
         <v>5.7</v>
       </c>
-      <c r="L26" s="42">
+      <c r="L26" s="16">
         <v>15.6</v>
       </c>
-      <c r="M26" s="46">
+      <c r="M26" s="20">
         <v>1.2</v>
       </c>
-      <c r="N26" s="42">
+      <c r="N26" s="16">
         <v>20.9</v>
       </c>
-      <c r="O26" s="43">
+      <c r="O26" s="17">
         <v>1.5</v>
       </c>
-      <c r="P26" s="42">
+      <c r="P26" s="16">
         <v>30.5</v>
       </c>
-      <c r="Q26" s="43">
+      <c r="Q26" s="17">
         <v>1.3</v>
       </c>
-      <c r="R26" s="46">
+      <c r="R26" s="20">
         <v>28.5</v>
       </c>
-      <c r="S26" s="46">
+      <c r="S26" s="20">
         <v>1.8</v>
       </c>
     </row>
     <row r="27" spans="1:19" ht="20.25" customHeight="1">
-      <c r="A27" s="41" t="s">
+      <c r="A27" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="B27" s="42">
+      <c r="B27" s="16">
         <v>31.5</v>
       </c>
-      <c r="C27" s="43">
+      <c r="C27" s="17">
         <v>4.3</v>
       </c>
-      <c r="D27" s="42">
+      <c r="D27" s="16">
         <v>28.8</v>
       </c>
-      <c r="E27" s="43">
+      <c r="E27" s="17">
         <v>4.5</v>
       </c>
-      <c r="F27" s="43">
+      <c r="F27" s="17">
         <v>35.6</v>
       </c>
-      <c r="G27" s="43">
+      <c r="G27" s="17">
         <v>4</v>
       </c>
-      <c r="H27" s="42">
+      <c r="H27" s="16">
         <v>41.9</v>
       </c>
-      <c r="I27" s="44">
+      <c r="I27" s="18">
         <v>4.3</v>
       </c>
-      <c r="J27" s="42">
+      <c r="J27" s="16">
         <v>47</v>
       </c>
-      <c r="K27" s="44">
+      <c r="K27" s="18">
         <v>3.9</v>
       </c>
-      <c r="L27" s="42">
+      <c r="L27" s="16">
         <v>20.8</v>
       </c>
-      <c r="M27" s="46">
+      <c r="M27" s="20">
         <v>4.7</v>
       </c>
-      <c r="N27" s="42">
+      <c r="N27" s="16">
         <v>25.3</v>
       </c>
-      <c r="O27" s="43">
+      <c r="O27" s="17">
         <v>4.0999999999999996</v>
       </c>
-      <c r="P27" s="42">
+      <c r="P27" s="16">
         <v>33.6</v>
       </c>
-      <c r="Q27" s="43">
+      <c r="Q27" s="17">
         <v>3.7</v>
       </c>
-      <c r="R27" s="46">
+      <c r="R27" s="20">
         <v>36.4</v>
       </c>
-      <c r="S27" s="46">
+      <c r="S27" s="20">
         <v>8.1999999999999993</v>
       </c>
     </row>
     <row r="28" spans="1:19" ht="20.25" customHeight="1">
-      <c r="A28" s="47" t="s">
+      <c r="A28" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="B28" s="48">
+      <c r="B28" s="22">
         <v>35.4</v>
       </c>
-      <c r="C28" s="49">
+      <c r="C28" s="23">
         <v>3.7</v>
       </c>
-      <c r="D28" s="48">
+      <c r="D28" s="22">
         <v>33</v>
       </c>
-      <c r="E28" s="49">
+      <c r="E28" s="23">
         <v>3.9</v>
       </c>
-      <c r="F28" s="49">
+      <c r="F28" s="23">
         <v>38.9</v>
       </c>
-      <c r="G28" s="49">
+      <c r="G28" s="23">
         <v>3.5</v>
       </c>
-      <c r="H28" s="48">
+      <c r="H28" s="22">
         <v>47.1</v>
       </c>
-      <c r="I28" s="50">
+      <c r="I28" s="24">
         <v>5.6</v>
       </c>
-      <c r="J28" s="48">
+      <c r="J28" s="22">
         <v>50.2</v>
       </c>
-      <c r="K28" s="50">
+      <c r="K28" s="24">
         <v>4.5</v>
       </c>
-      <c r="L28" s="48">
+      <c r="L28" s="22">
         <v>24.1</v>
       </c>
-      <c r="M28" s="51">
+      <c r="M28" s="25">
         <v>2.7</v>
       </c>
-      <c r="N28" s="48">
+      <c r="N28" s="22">
         <v>28.5</v>
       </c>
-      <c r="O28" s="49">
+      <c r="O28" s="23">
         <v>2.4</v>
       </c>
-      <c r="P28" s="48">
+      <c r="P28" s="22">
         <v>40.4</v>
       </c>
-      <c r="Q28" s="49">
+      <c r="Q28" s="23">
         <v>5.8</v>
       </c>
-      <c r="R28" s="51">
+      <c r="R28" s="25">
         <v>37.5</v>
       </c>
-      <c r="S28" s="51">
+      <c r="S28" s="25">
         <v>4.7</v>
+      </c>
+    </row>
+    <row r="29" spans="1:19">
+      <c r="A29" s="52">
+        <v>45017</v>
+      </c>
+      <c r="B29" s="1">
+        <v>36.4</v>
+      </c>
+      <c r="C29" s="1">
+        <v>2.4</v>
+      </c>
+      <c r="D29" s="1">
+        <v>33.5</v>
+      </c>
+      <c r="E29" s="1">
+        <v>2</v>
+      </c>
+      <c r="F29" s="1">
+        <v>40.700000000000003</v>
+      </c>
+      <c r="G29" s="1">
+        <v>3</v>
+      </c>
+      <c r="H29" s="1">
+        <v>46.8</v>
+      </c>
+      <c r="I29" s="1">
+        <v>3.4</v>
+      </c>
+      <c r="J29" s="1">
+        <v>52.2</v>
+      </c>
+      <c r="K29" s="1">
+        <v>4.2</v>
+      </c>
+      <c r="L29" s="1">
+        <v>24.9</v>
+      </c>
+      <c r="M29" s="1">
+        <v>1</v>
+      </c>
+      <c r="N29" s="1">
+        <v>29.9</v>
+      </c>
+      <c r="O29" s="1">
+        <v>1.6</v>
+      </c>
+      <c r="P29" s="1">
+        <v>42.1</v>
+      </c>
+      <c r="Q29" s="1">
+        <v>2.7</v>
+      </c>
+      <c r="R29" s="1">
+        <v>32.799999999999997</v>
+      </c>
+      <c r="S29" s="1">
+        <v>-0.4</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="F5:G5"/>
-    <mergeCell ref="H5:I5"/>
-    <mergeCell ref="J5:K5"/>
-    <mergeCell ref="L5:M5"/>
-    <mergeCell ref="N5:O5"/>
     <mergeCell ref="A1:T1"/>
     <mergeCell ref="A2:S2"/>
     <mergeCell ref="B3:O3"/>
@@ -3013,7 +3073,13 @@
     <mergeCell ref="L4:O4"/>
     <mergeCell ref="B5:C5"/>
     <mergeCell ref="D5:E5"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="H5:I5"/>
+    <mergeCell ref="J5:K5"/>
+    <mergeCell ref="L5:M5"/>
+    <mergeCell ref="N5:O5"/>
   </mergeCells>
+  <phoneticPr fontId="16" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>